<commit_message>
Added non infected seeders to susceptibles
</commit_message>
<xml_diff>
--- a/Appendix_individualsCtvaluesandevaluation.xlsx
+++ b/Appendix_individualsCtvaluesandevaluation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Surfdrive\Models_and_Scripts\TransmissionExperiment\TransmissionEstimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D222DD-3895-4795-A605-FE9C24B4926C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7D3405-7B91-4F89-9AD8-B60ADA5F1AA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -460,7 +460,119 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -835,8 +947,8 @@
   </sheetPr>
   <dimension ref="B1:W240"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B242" sqref="B242"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G167" sqref="G167:T167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13181,16 +13293,16 @@
     <mergeCell ref="C51:C86"/>
   </mergeCells>
   <conditionalFormatting sqref="G3:U233">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
       <formula>"NI"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" operator="equal">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>"I"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>